<commit_message>
Removed Old File and Added Call Notes
-Removed old team.md file
-Added notes from call with Ryan.
</commit_message>
<xml_diff>
--- a/docs/responsibility_chart.xlsx
+++ b/docs/responsibility_chart.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dwfp-my.sharepoint.com/personal/ashehadeh_dwfp_com/Documents/Lewis/Capstone/h2o/docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\atodev\Documents\Private\h2o\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="8_{6D4C4C84-ACEA-4ECC-B1D1-2A53D1D8F139}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{B9225556-BCBB-446A-BA64-347EDF9C39DC}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{810D54A5-3291-4A98-8BCD-5170744D6672}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17985" windowHeight="5850" xr2:uid="{E6D26986-00E4-4126-9AC0-2B652C66D5C3}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="179021"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="25">
   <si>
     <t>Task</t>
   </si>
@@ -100,6 +99,12 @@
   </si>
   <si>
     <t>Complete login system</t>
+  </si>
+  <si>
+    <t>Reach out to business</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
@@ -143,10 +148,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -461,20 +472,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C7A2352-F871-41FB-98CD-18934B7834E3}">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="124" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="62.19921875" customWidth="1"/>
-    <col min="2" max="2" width="15.9296875" customWidth="1"/>
-    <col min="3" max="3" width="18.265625" customWidth="1"/>
+    <col min="1" max="1" width="62.140625" customWidth="1"/>
+    <col min="2" max="2" width="16" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -484,11 +496,11 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -498,11 +510,11 @@
       <c r="C2" s="2">
         <v>43369</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -512,11 +524,11 @@
       <c r="C3" s="2">
         <v>43373</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -526,11 +538,11 @@
       <c r="C4" s="2">
         <v>43375</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -538,7 +550,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -546,7 +558,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -554,83 +566,115 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>22</v>
       </c>
       <c r="B8" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="C8" s="2">
+        <v>43394</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="2">
+        <v>43393</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>6</v>
       </c>
-      <c r="B9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A10" t="s">
+      <c r="B10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="2">
+        <v>43396</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>17</v>
       </c>
-      <c r="B10" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A11" t="s">
+      <c r="B11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>5</v>
       </c>
-      <c r="B11" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A12" t="s">
+      <c r="B12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="2">
+        <v>43399</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>13</v>
       </c>
-      <c r="B12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A13" t="s">
+      <c r="B13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>8</v>
       </c>
-      <c r="B13" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A14" t="s">
+      <c r="B14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>9</v>
       </c>
-      <c r="B14" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A15" t="s">
+      <c r="B15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>10</v>
       </c>
-      <c r="B15" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A16" t="s">
+      <c r="B16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>11</v>
       </c>
-      <c r="B16" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A17" t="s">
+      <c r="B17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>12</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B18" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated ER_Diagram and responsibility chart
</commit_message>
<xml_diff>
--- a/docs/responsibility_chart.xlsx
+++ b/docs/responsibility_chart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AShehadeh\OneDrive - D&amp;W Fine Pack\Lewis\Capstone\h2o\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="21" documentId="102_{A0587E3E-3D0E-4BF8-B69A-FF530DD07D53}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{20AE01A1-4C88-4B79-A52E-96C5B00A9F6E}"/>
+  <xr:revisionPtr revIDLastSave="60" documentId="102_{A0587E3E-3D0E-4BF8-B69A-FF530DD07D53}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{1F38120C-DDFD-47A8-9AAC-81EFA49F48D5}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17985" windowHeight="5850" activeTab="1" xr2:uid="{E6D26986-00E4-4126-9AC0-2B652C66D5C3}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17985" windowHeight="5850" xr2:uid="{E6D26986-00E4-4126-9AC0-2B652C66D5C3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="41">
   <si>
     <t>Task</t>
   </si>
@@ -42,9 +42,6 @@
     <t>Completion Date</t>
   </si>
   <si>
-    <t>Done</t>
-  </si>
-  <si>
     <t>Create multi-dimensional database</t>
   </si>
   <si>
@@ -87,9 +84,6 @@
     <t>Create staff information page with picture and other user information</t>
   </si>
   <si>
-    <t>X</t>
-  </si>
-  <si>
     <t>Create new cloudsite to debug code against (with PHP and MySQL)</t>
   </si>
   <si>
@@ -103,9 +97,6 @@
   </si>
   <si>
     <t>Reach out to business</t>
-  </si>
-  <si>
-    <t>x</t>
   </si>
   <si>
     <t>Dashboard – Fix recent surveys window rendering. Ask Ryan what we should do to this page?</t>
@@ -258,12 +249,18 @@
   <si>
     <t>Plans per page:</t>
   </si>
+  <si>
+    <t>Waiting on</t>
+  </si>
+  <si>
+    <t>In Progress</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -293,13 +290,37 @@
       <name val="Calibri Light"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -311,10 +332,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -333,8 +356,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Bad" xfId="1" builtinId="27"/>
+    <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -649,8 +676,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C7A2352-F871-41FB-98CD-18934B7834E3}">
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="124" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" zoomScale="124" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -671,242 +698,270 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="D1" s="3"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C2" s="2">
         <v>43369</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>18</v>
-      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C3" s="2">
         <v>43373</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>18</v>
-      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C4" s="2">
         <v>43375</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>18</v>
-      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>18</v>
+      </c>
+      <c r="C5" s="2">
+        <v>43408</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>19</v>
+      </c>
+      <c r="C6" s="2">
+        <v>43410</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>18</v>
+      </c>
+      <c r="C7" s="2">
+        <v>43411</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C8" s="2">
         <v>43394</v>
       </c>
-      <c r="D8" s="4" t="s">
-        <v>24</v>
-      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C9" s="2">
         <v>43393</v>
       </c>
-      <c r="D9" s="4" t="s">
-        <v>24</v>
-      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C10" s="2">
         <v>43396</v>
       </c>
-      <c r="D10" s="4" t="s">
-        <v>24</v>
-      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
+        <v>18</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C12" s="2">
         <v>43399</v>
       </c>
-      <c r="D12" s="4" t="s">
-        <v>24</v>
-      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>21</v>
+        <v>19</v>
+      </c>
+      <c r="C13" s="2">
+        <v>43416</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B14" t="s">
-        <v>20</v>
+        <v>18</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B15" t="s">
-        <v>21</v>
+        <v>19</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>10</v>
       </c>
-      <c r="B16" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="B17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>11</v>
       </c>
-      <c r="B17" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>12</v>
-      </c>
       <c r="B18" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
+      <c r="B22" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B20" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
+      <c r="B23" t="s">
+        <v>19</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B21" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
+      <c r="B24" t="s">
+        <v>18</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B22" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B23" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="B24" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="6" t="s">
-        <v>33</v>
-      </c>
       <c r="B25" t="s">
-        <v>20</v>
+        <v>18</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -919,7 +974,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{474706BF-9DC6-4043-B6B6-CFB0AB1A7A93}">
   <dimension ref="A2:A17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
@@ -927,37 +982,37 @@
   <sheetData>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
@@ -965,42 +1020,42 @@
     </row>
     <row r="10" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adam & angel fall 2018
</commit_message>
<xml_diff>
--- a/docs/responsibility_chart.xlsx
+++ b/docs/responsibility_chart.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AShehadeh\OneDrive - D&amp;W Fine Pack\Lewis\Capstone\h2o\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adam\OneDrive - D&amp;W Fine Pack\Lewis\Capstone\h2o\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="60" documentId="102_{A0587E3E-3D0E-4BF8-B69A-FF530DD07D53}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{1F38120C-DDFD-47A8-9AAC-81EFA49F48D5}"/>
+  <xr:revisionPtr revIDLastSave="73" documentId="102_{A0587E3E-3D0E-4BF8-B69A-FF530DD07D53}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{3EB69385-B89E-483D-B5AA-52DCF1C13AC4}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17985" windowHeight="5850" xr2:uid="{E6D26986-00E4-4126-9AC0-2B652C66D5C3}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="39">
   <si>
     <t>Task</t>
   </si>
@@ -249,18 +249,12 @@
   <si>
     <t>Plans per page:</t>
   </si>
-  <si>
-    <t>Waiting on</t>
-  </si>
-  <si>
-    <t>In Progress</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -290,37 +284,13 @@
       <name val="Calibri Light"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -332,12 +302,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -356,12 +324,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="Bad" xfId="1" builtinId="27"/>
-    <cellStyle name="Good" xfId="2" builtinId="26"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -676,19 +640,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C7A2352-F871-41FB-98CD-18934B7834E3}">
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="124" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="124" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="85.140625" customWidth="1"/>
+    <col min="1" max="1" width="85.1328125" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="3" max="3" width="18.28515625" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="4"/>
+    <col min="3" max="3" width="18.265625" customWidth="1"/>
+    <col min="4" max="4" width="9.1328125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -700,7 +664,7 @@
       </c>
       <c r="D1" s="3"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -711,7 +675,7 @@
         <v>43369</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -722,7 +686,7 @@
         <v>43373</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -733,7 +697,7 @@
         <v>43375</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -744,7 +708,7 @@
         <v>43408</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -755,7 +719,7 @@
         <v>43410</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -766,7 +730,7 @@
         <v>43411</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -777,7 +741,7 @@
         <v>43394</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -788,7 +752,7 @@
         <v>43393</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -799,18 +763,18 @@
         <v>43396</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>16</v>
       </c>
       <c r="B11" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="9" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C11" s="2">
+        <v>43435</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -821,7 +785,7 @@
         <v>43399</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -832,136 +796,136 @@
         <v>43416</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>7</v>
       </c>
       <c r="B14" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="9" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C14" s="2">
+        <v>43435</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>8</v>
       </c>
       <c r="B15" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="9" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C15" s="2">
+        <v>43435</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>9</v>
       </c>
       <c r="B16" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="9" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C16" s="2">
+        <v>43435</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>10</v>
       </c>
       <c r="B17" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="9" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C17" s="2">
+        <v>43435</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>11</v>
       </c>
       <c r="B18" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="9" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C18" s="2">
+        <v>43435</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A19" s="5" t="s">
         <v>24</v>
       </c>
       <c r="B19" t="s">
         <v>18</v>
       </c>
-      <c r="C19" s="8" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C19" s="2">
+        <v>43421</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A20" s="5" t="s">
         <v>25</v>
       </c>
       <c r="B20" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="8" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C20" s="2">
+        <v>43422</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A21" s="6" t="s">
         <v>26</v>
       </c>
       <c r="B21" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="8" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C21" s="2">
+        <v>43423</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A22" s="6" t="s">
         <v>27</v>
       </c>
       <c r="B22" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="8" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C22" s="2">
+        <v>43424</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A23" s="6" t="s">
         <v>28</v>
       </c>
       <c r="B23" t="s">
         <v>19</v>
       </c>
-      <c r="C23" s="8" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C23" s="2">
+        <v>43425</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A24" s="6" t="s">
         <v>29</v>
       </c>
       <c r="B24" t="s">
         <v>18</v>
       </c>
-      <c r="C24" s="8" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C24" s="2">
+        <v>43423</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A25" s="6" t="s">
         <v>30</v>
       </c>
       <c r="B25" t="s">
         <v>18</v>
       </c>
-      <c r="C25" s="8" t="s">
-        <v>39</v>
+      <c r="C25" s="2">
+        <v>43423</v>
       </c>
     </row>
   </sheetData>
@@ -978,82 +942,82 @@
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A2" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A3" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A4" s="5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A5" s="5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A6" s="5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A7" s="5" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A8" s="5" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A9" s="5"/>
     </row>
-    <row r="10" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" ht="16.899999999999999" x14ac:dyDescent="0.45">
       <c r="A10" s="7" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A11" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A12" s="5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A13" s="6" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A14" s="6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A15" s="6" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A16" s="6" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A17" s="6" t="s">
         <v>30</v>
       </c>

</xml_diff>